<commit_message>
Update master sheet functionality to properly map data from uploaded Excel sheets to corresponding columns, and fix data extraction logic
</commit_message>
<xml_diff>
--- a/master_attendance_summary.xlsx
+++ b/master_attendance_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c5efb8c331beb78/induction auto mail(2)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="11_290E2653C62EF150E33DC131F763D66E6B6EB3D2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2862003-99DA-4D16-91B7-F3F7F67A9690}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_61DAA640C62EF1806A7B3DF689A6C0A86B6E13EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FE406A9-D995-45B0-8824-3F3B090D9F2D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="47">
   <si>
     <t>Sr No</t>
   </si>
@@ -34,15 +34,12 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>Batch No</t>
-  </si>
-  <si>
-    <t>Grade</t>
-  </si>
-  <si>
     <t>Induction Month</t>
   </si>
   <si>
+    <t>Induction Week</t>
+  </si>
+  <si>
     <t>Induction Start Date</t>
   </si>
   <si>
@@ -77,6 +74,93 @@
   </si>
   <si>
     <t>Shop</t>
+  </si>
+  <si>
+    <t>11202797</t>
+  </si>
+  <si>
+    <t>SIDDHARAM KALYANI SHINDE</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>11202798</t>
+  </si>
+  <si>
+    <t>NIRAJ NETAJI BHATLAWANDE</t>
+  </si>
+  <si>
+    <t>11202799</t>
+  </si>
+  <si>
+    <t>PARTH SANJAY KARVEKAR</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>11202800</t>
+  </si>
+  <si>
+    <t>SUJAL SUNIL BHUSANE</t>
+  </si>
+  <si>
+    <t>11202801</t>
+  </si>
+  <si>
+    <t>NAMRATA ASHOKARAO PATIL</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>11202802</t>
+  </si>
+  <si>
+    <t>RAHUL SANJAY MORE</t>
+  </si>
+  <si>
+    <t>11202803</t>
+  </si>
+  <si>
+    <t>AKASH VILAS PAWAR</t>
+  </si>
+  <si>
+    <t>11202804</t>
+  </si>
+  <si>
+    <t>POOJA RAMESH JADHAV</t>
+  </si>
+  <si>
+    <t>11202805</t>
+  </si>
+  <si>
+    <t>ROHIT ANIL DESHMUKH</t>
+  </si>
+  <si>
+    <t>11202806</t>
+  </si>
+  <si>
+    <t>KIRAN MAHESH PATIL</t>
+  </si>
+  <si>
+    <t>11202807</t>
+  </si>
+  <si>
+    <t>SNEHA VIKAS SHINDE</t>
+  </si>
+  <si>
+    <t>11202808</t>
+  </si>
+  <si>
+    <t>VIVEK RAVINDRA JOSHI</t>
   </si>
 </sst>
 </file>
@@ -97,18 +181,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,7 +203,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,28 +522,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" customWidth="1"/>
-    <col min="11" max="11" width="19.109375" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="19" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" customWidth="1"/>
-    <col min="16" max="16" width="17.77734375" customWidth="1"/>
-    <col min="17" max="17" width="16.88671875" customWidth="1"/>
-    <col min="18" max="18" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,8 +600,1349 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>21</v>
+      </c>
+      <c r="R6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>21</v>
+      </c>
+      <c r="R8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>21</v>
+      </c>
+      <c r="R10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>21</v>
+      </c>
+      <c r="R11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>21</v>
+      </c>
+      <c r="R12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" t="s">
+        <v>21</v>
+      </c>
+      <c r="P13" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>21</v>
+      </c>
+      <c r="R13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>21</v>
+      </c>
+      <c r="R14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15" t="s">
+        <v>21</v>
+      </c>
+      <c r="P15" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>21</v>
+      </c>
+      <c r="R15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" t="s">
+        <v>21</v>
+      </c>
+      <c r="P16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>21</v>
+      </c>
+      <c r="R16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O17" t="s">
+        <v>21</v>
+      </c>
+      <c r="P17" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>21</v>
+      </c>
+      <c r="R17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" t="s">
+        <v>21</v>
+      </c>
+      <c r="N18" t="s">
+        <v>21</v>
+      </c>
+      <c r="O18" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>21</v>
+      </c>
+      <c r="R18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" t="s">
+        <v>21</v>
+      </c>
+      <c r="N19" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" t="s">
+        <v>21</v>
+      </c>
+      <c r="P20" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>21</v>
+      </c>
+      <c r="R20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21" t="s">
+        <v>21</v>
+      </c>
+      <c r="O21" t="s">
+        <v>21</v>
+      </c>
+      <c r="P21" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>21</v>
+      </c>
+      <c r="R21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N22" t="s">
+        <v>21</v>
+      </c>
+      <c r="O22" t="s">
+        <v>21</v>
+      </c>
+      <c r="P22" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>21</v>
+      </c>
+      <c r="R22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" t="s">
+        <v>21</v>
+      </c>
+      <c r="N23" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" t="s">
+        <v>21</v>
+      </c>
+      <c r="P23" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>21</v>
+      </c>
+      <c r="R23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M24" t="s">
+        <v>21</v>
+      </c>
+      <c r="N24" t="s">
+        <v>21</v>
+      </c>
+      <c r="O24" t="s">
+        <v>21</v>
+      </c>
+      <c r="P24" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>21</v>
+      </c>
+      <c r="R24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" t="s">
+        <v>21</v>
+      </c>
+      <c r="M25" t="s">
+        <v>21</v>
+      </c>
+      <c r="N25" t="s">
+        <v>21</v>
+      </c>
+      <c r="O25" t="s">
+        <v>21</v>
+      </c>
+      <c r="P25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R25" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>